<commit_message>
added info on additional costs and new templates
</commit_message>
<xml_diff>
--- a/template/apc_template.xlsx
+++ b/template/apc_template.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camlin\system\openapc-se\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2021m30/R/repos/openapc-se/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68FA9E6-52FA-974B-AD65-BF7A1138B076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38055" windowHeight="23265" tabRatio="500"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="38060" windowHeight="23260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="article data" sheetId="1" r:id="rId1"/>
+    <sheet name="additional costs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="template" localSheetId="0">Blad1!$A$1:$K$2</definedName>
+    <definedName name="template" localSheetId="0">'article data'!$A$1:$K$2</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -30,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="template" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="template" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/ulfkro/OneDrive/KB-dokument/Open Access/Kostnader/Open APC Sweden/openapc-se/template/template.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>institution</t>
   </si>
@@ -86,12 +88,39 @@
   <si>
     <t>sek</t>
   </si>
+  <si>
+    <t>colour charge</t>
+  </si>
+  <si>
+    <t>cover charge</t>
+  </si>
+  <si>
+    <t>page charge</t>
+  </si>
+  <si>
+    <t>permission</t>
+  </si>
+  <si>
+    <t>reprint</t>
+  </si>
+  <si>
+    <t>submission fee</t>
+  </si>
+  <si>
+    <t>payment fee</t>
+  </si>
+  <si>
+    <t>other 1</t>
+  </si>
+  <si>
+    <t>other 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,9 +132,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,9 +162,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,7 +184,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="template" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="template" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,61 +449,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E9D608-332C-6B41-B918-E0AD75CD6855}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>